<commit_message>
additional models and submissions
</commit_message>
<xml_diff>
--- a/Model performance.xlsx
+++ b/Model performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21435" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="21435" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="External" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
     <sheet name="Selected covs" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="230">
   <si>
     <t>Date</t>
   </si>
@@ -651,6 +652,24 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color theme="4" tint="0.39997558519241921"/>
         <rFont val="Lucida Console"/>
         <family val="3"/>
@@ -664,11 +683,130 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
+      <t xml:space="preserve"> + Q116953 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q121699</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q102089</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
       <t xml:space="preserve"> + </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115899</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color theme="7" tint="-0.249977111117893"/>
         <rFont val="Lucida Console"/>
         <family val="3"/>
@@ -682,11 +820,94 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
+      <t xml:space="preserve"> +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Q98869</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
       <t xml:space="preserve"> + </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q121699</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color theme="7" tint="0.59999389629810485"/>
         <rFont val="Lucida Console"/>
         <family val="3"/>
@@ -700,12 +921,414 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q102089</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q124122 + Gender + Q108754 + Q100680 + Q98078 + Q116953 + Q106272 + Q123621 + Q101162 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q98869</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q118232</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q121699</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q102089</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Gender + Q118232 + Q116953 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q98869</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q106272 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115899</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q121699</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q102089</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Gender + Q108754 + Q101162 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q98869</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q116953 + Q106272 + Q123621 + Q118232 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115899</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q121699</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
       <t xml:space="preserve"> + Gender + </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
@@ -752,6 +1375,42 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q121699</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color theme="7" tint="0.59999389629810485"/>
         <rFont val="Lucida Console"/>
         <family val="3"/>
@@ -770,6 +1429,164 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q102089</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q124122 + Gender + Q98078 + Q100680 + Q116953 + Q106272 + Q118232 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115899</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q98869</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HouseholdStatus + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q102089</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q110740 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115899</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color theme="4" tint="0.39997558519241921"/>
         <rFont val="Lucida Console"/>
         <family val="3"/>
@@ -783,7 +1600,192 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> + Q116953 + </t>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9933FF"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q120379</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q98869</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q99480 + YOB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HouseholdStatus + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q102089</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q110740 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115899</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9933FF"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q120379</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
     </r>
     <r>
       <rPr>
@@ -794,10 +1796,55 @@
       </rPr>
       <t>Q121699</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">HouseholdStatus + Q101163 + </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q98869</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q99480 + YOB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HouseholdStatus + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q107869 + Q108342 + </t>
     </r>
     <r>
       <rPr>
@@ -833,11 +1880,124 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
+      <t xml:space="preserve"> + Q115195 + Q115390 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
       <t xml:space="preserve"> + </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q116953 + Q120194 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9933FF"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q120379</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q120472 + Q122771 + Q123621 + Q99480 + YOB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HouseholdStatus + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q109244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q110740 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color theme="7" tint="0.59999389629810485"/>
         <rFont val="Lucida Console"/>
         <family val="3"/>
@@ -874,6 +2034,291 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">YOB + HouseholdStatus + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9933FF"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q120379</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q120472 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q110740 + Q109244 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q99480 + Q108342 + Q115195 + Q120194 + Q122771</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">YOB + HouseholdStatus + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9933FF"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q120379</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q120472 + Q119851 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q110740 + Q109244 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q99480 + Q108342 + Q108855 + Q108856 + Q115195 + Q120194 + Q122771 + Q123621</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">YOB + HouseholdStatus + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF9933FF"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q120379</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q120472 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q116881</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q115611</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q113181</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q110740 + Q109244 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + Q99480</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">YOB + HouseholdStatus + Q122771 + </t>
     </r>
     <r>
@@ -910,21 +2355,16 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> + Q115390 + Q115195 + Q113181 + Q110740 + Q109244 + Q108342 + Q107869 + Q101163 + Q99480 + Q98197</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">YOB + HouseholdStatus + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF9933FF"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q120379</t>
+      <t xml:space="preserve"> + Q115390 + Q115195 + Q113181 + Q110740 + Q109244 + Q108342 + Q107869 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF339933"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Q101163</t>
     </r>
     <r>
       <rPr>
@@ -933,1310 +2373,72 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> + Q120472 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q110740 + Q109244 + Q101163 + Q99480</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">YOB + HouseholdStatus + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF9933FF"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q120379</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q120472 + Q119851 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q110740 + Q109244 + Q101163 + Q99480 + Q108342 + Q108855 + Q108856 + Q115195 + Q120194 + Q122771 + Q123621</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">YOB + HouseholdStatus + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF9933FF"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q120379</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q120472 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q110740 + Q109244 + Q101163 + Q99480 + Q108342 + Q115195 + Q120194 + Q122771</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">HouseholdStatus + Q101163 + Q107869 + Q108342 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q110740 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q115195 + Q115390 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q116953 + Q120194 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF9933FF"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q120379</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q120472 + Q122771 + Q123621 + Q99480 + YOB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q102089</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115899</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q121699</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q98869</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">HouseholdStatus + Q101163 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q102089</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q110740 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115899</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF9933FF"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q120379</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q98869</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q99480 + YOB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">HouseholdStatus + Q101163 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q102089</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q110740 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115899</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF9933FF"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q120379</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q121699</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q98869</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q99480 + YOB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q121699</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q102089</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q124122 + Gender + Q108754 + Q100680 + Q98078 + Q116953 + Q106272 + Q123621 + Q101162 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q98869</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q118232</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q121699</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q102089</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Gender + Q118232 + Q116953 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q98869</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q106272 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115899</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q121699</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q102089</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Gender + Q108754 + Q101162 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q98869</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q116953 + Q106272 + Q123621 + Q118232 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115899</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q109244</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q113181</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="0.39997558519241921"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q116881</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q121699</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q102089</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + Q124122 + Gender + Q98078 + Q100680 + Q116953 + Q106272 + Q118232 + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="6" tint="0.59999389629810485"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q115899</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Q98869</t>
-    </r>
+      <t xml:space="preserve"> + Q99480 + Q98197</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Q102089 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HouseholdStatus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q101163 </t>
+  </si>
+  <si>
+    <t>SigPlus</t>
+  </si>
+  <si>
+    <t>Q105840</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>* good book</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>EducationLevel</t>
+  </si>
+  <si>
+    <t>Q104996</t>
+  </si>
+  <si>
+    <t>gbmSeln</t>
+  </si>
+  <si>
+    <t>gbm5</t>
+  </si>
+  <si>
+    <t>gbm</t>
+  </si>
+  <si>
+    <t>may have overwritten previous rf7; default settings in cforest/party package</t>
+  </si>
+  <si>
+    <t>rf8</t>
+  </si>
+  <si>
+    <t>as above with ntree and mtry adjusted</t>
+  </si>
+  <si>
+    <t>cov_sigQplus, "Income", "EducationLevel"</t>
+  </si>
+  <si>
+    <t>rf9</t>
+  </si>
+  <si>
+    <t>&lt;0.49, otherwise as rf8 where threshold was 0.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2360,12 +2562,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF9933FF"/>
       <name val="Lucida Console"/>
       <family val="3"/>
@@ -2375,6 +2571,57 @@
       <color rgb="FF66FF33"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF339933"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF339933"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF339933"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2397,7 +2644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2430,6 +2677,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2486,6 +2741,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF339933"/>
       <color rgb="FF66FF33"/>
     </mruColors>
   </colors>
@@ -2784,10 +3040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3267,6 +3523,103 @@
         <v>195</v>
       </c>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>42534</v>
+      </c>
+      <c r="B26" t="s">
+        <v>222</v>
+      </c>
+      <c r="C26">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="D26" t="s">
+        <v>186</v>
+      </c>
+      <c r="E26" t="s">
+        <v>223</v>
+      </c>
+      <c r="F26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="D27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" t="s">
+        <v>176</v>
+      </c>
+      <c r="G27" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>225</v>
+      </c>
+      <c r="C28">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="D28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>225</v>
+      </c>
+      <c r="C29">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="D29" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C30">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="D30" t="s">
+        <v>186</v>
+      </c>
+      <c r="E30" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" t="s">
+        <v>227</v>
+      </c>
+      <c r="G30" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3276,8 +3629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3332,7 +3685,7 @@
         <v>glm3backwards selection</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3353,7 +3706,7 @@
         <v>glm3forwards selection</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="I5" s="17"/>
     </row>
@@ -3391,7 +3744,7 @@
         <v>glm4backwards selection</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3412,7 +3765,7 @@
         <v>glm4forwards selection</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3443,7 +3796,7 @@
         <v>glm5backwards selection</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3464,7 +3817,7 @@
         <v>glm5forwards selection</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3498,7 +3851,7 @@
         <v>glm6backwards selection</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3519,7 +3872,7 @@
         <v>glm6forwards selection</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -3558,7 +3911,7 @@
         <v>glm7backwards selection</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3579,7 +3932,7 @@
         <v>glm7forwards selection</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -3618,7 +3971,7 @@
         <v>glm8backwards selection</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -3676,7 +4029,7 @@
         <v>glm9backwards selection</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3697,7 +4050,7 @@
         <v>glm9forwards selection</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -3715,7 +4068,7 @@
         <v>glm13</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -3733,7 +4086,7 @@
         <v>glm14</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -3751,7 +4104,7 @@
         <v>glm15</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -3773,7 +4126,7 @@
   <dimension ref="A1:DC16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8443,10 +8796,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8456,7 +8809,7 @@
     <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -8466,129 +8819,222 @@
       <c r="C1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="19" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="21" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>83</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="21" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="19" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="21" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>88</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="19" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>89</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
+        <v>216</v>
+      </c>
+      <c r="F10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>90</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="19" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>91</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="19" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -8598,119 +9044,176 @@
       <c r="C13" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>93</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>94</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="21" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="21" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="19" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="19" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -8731,9 +9234,109 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="C3:C35">
-    <sortCondition ref="C3:C35"/>
+  <sortState ref="D2:D35">
+    <sortCondition ref="D2:D35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>